<commit_message>
Eliminated blank rows at end of data
</commit_message>
<xml_diff>
--- a/data/hospital_infections.xlsx
+++ b/data/hospital_infections.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10D8FCE-11BC-45E2-BEE8-CABDFF9BB952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A9DF64-13ED-41F8-9800-F0D1870BB78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="90">
   <si>
     <t>Pair 01</t>
   </si>
@@ -678,11 +678,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1422,26 +1420,6 @@
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D56" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D57" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>